<commit_message>
[#641] SchemaOCDS: get rid of get_extended_release_schema_url and instead encapsulate that logic in refactored create_extended_release_schema_file
</commit_message>
<xml_diff>
--- a/cove_ocds/fixtures/tenders_releases_2_releases_with_metatab_and_extensions.xlsx
+++ b/cove_ocds/fixtures/tenders_releases_2_releases_with_metatab_and_extensions.xlsx
@@ -276,7 +276,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.4736842105263"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="15.8016194331984"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -411,10 +411,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4736842105263"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.6558704453441"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.7935222672065"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="14.4736842105263"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8016194331984"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.8906882591093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.9352226720648"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="15.8016194331984"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -594,10 +594,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4736842105263"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.8987854251012"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.8502024291498"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="14.4736842105263"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8016194331984"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.748987854251"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.8906882591093"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="15.8016194331984"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -688,16 +688,16 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D47" activeCellId="0" sqref="D47"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.3238866396761"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="162.720647773279"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.6153846153846"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="34.0931174089069"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="17.3238866396761"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.9473684210526"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="178.437246963563"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.9028340080972"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="37.3279352226721"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="18.9473684210526"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -718,7 +718,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://raw.githubusercontent.com/open-contracting/ocds_metrics_extension/master/extension.json"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://raw.githubusercontent.com/open-contracting/ocds_metrics_extension/master/extension.json; https://raw.githubusercontent.com/open-contracting/ocds_extension_parties/master/extension.json;   https://raw.githubusercontent.com/open-contracting/ocds_partyDetails_scale_extension/master/extension.json"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>